<commit_message>
Commit for latest update
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData.xlsx
+++ b/src/test/resources/TestData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PScope\eclipse-workspace\JD_SeleniumFramework\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3DF42FD5-33E8-4D32-88EE-73AA88E0EDD8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4CC59C56-7C69-45AF-8EB4-9309B0A5579B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,13 +34,13 @@
     <t>Admin</t>
   </si>
   <si>
-    <t>Admin123</t>
-  </si>
-  <si>
     <t>Username</t>
   </si>
   <si>
     <t>Jitendra123</t>
+  </si>
+  <si>
+    <t>admin123</t>
   </si>
 </sst>
 </file>
@@ -379,7 +379,7 @@
   <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -390,7 +390,7 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
@@ -401,7 +401,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.35">
@@ -409,7 +409,7 @@
         <v>1</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>